<commit_message>
Dodano wyniki McCornic i TSP
</commit_message>
<xml_diff>
--- a/Programowanie/Sztuczna_inteligencja/problemy_i_implementacja/wyniki/Wyniki.xlsx
+++ b/Programowanie/Sztuczna_inteligencja/problemy_i_implementacja/wyniki/Wyniki.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bb75cf0a1a68a1d/Materiały pisane/Blog/Programowanie/Sztuczna_inteligencja/problemy_i_implementacja/wyniki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{28B68594-DEBB-4325-9A73-A8DA43E1A7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{28B68594-DEBB-4325-9A73-A8DA43E1A7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{381EC865-4791-4914-839B-71C1449EF66F}"/>
   <bookViews>
-    <workbookView xWindow="37785" yWindow="0" windowWidth="12600" windowHeight="21600" activeTab="1" xr2:uid="{9D055064-E54F-488C-B0AE-076216540D4E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="50625" windowHeight="21840" activeTab="3" xr2:uid="{9D055064-E54F-488C-B0AE-076216540D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Knapsack" sheetId="1" r:id="rId1"/>
     <sheet name="Schfew" sheetId="2" r:id="rId2"/>
+    <sheet name="McCornic" sheetId="3" r:id="rId3"/>
+    <sheet name="TSP" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="59">
   <si>
     <t>CrossoverName</t>
   </si>
@@ -85,31 +87,142 @@
     <t>TheSameNeuronWinner</t>
   </si>
   <si>
-    <t>Suma</t>
-  </si>
-  <si>
-    <t>Średnia</t>
-  </si>
-  <si>
-    <t>Suma bieżąca</t>
-  </si>
-  <si>
-    <t>Liczba</t>
-  </si>
-  <si>
-    <t>Kolumna1</t>
-  </si>
-  <si>
     <t>Crossover.Ratio</t>
   </si>
   <si>
     <t>UniformCrossover`2</t>
+  </si>
+  <si>
+    <t>_id.$oid</t>
+  </si>
+  <si>
+    <t>SelectionName</t>
+  </si>
+  <si>
+    <t>Selection.IsReversed</t>
+  </si>
+  <si>
+    <t>Selection.HasMinus</t>
+  </si>
+  <si>
+    <t>WinnerChromosome.Fitness</t>
+  </si>
+  <si>
+    <t>RealTheBestValue</t>
+  </si>
+  <si>
+    <t>TheBestFoundFitness</t>
+  </si>
+  <si>
+    <t>Steps.generation</t>
+  </si>
+  <si>
+    <t>Steps.Elapse</t>
+  </si>
+  <si>
+    <t>Steps.fitness</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>RouletteSelection</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>UniformCrossover</t>
+  </si>
+  <si>
+    <t>SwapMutation</t>
+  </si>
+  <si>
+    <t>Termination.AmountLastNeruonWins</t>
+  </si>
+  <si>
+    <t>WinnerChromosome.TotalPath</t>
+  </si>
+  <si>
+    <t>60aa255675968d07c7f04735</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>60aad6098b49bd016e0fb99e</t>
+  </si>
+  <si>
+    <t>60aa255675968d07c7f047b7</t>
+  </si>
+  <si>
+    <t>60aad6098b49bd016e0fb8e8</t>
+  </si>
+  <si>
+    <t>60aad6098b49bd016e0fb819</t>
+  </si>
+  <si>
+    <t>60aad5c85cdac2016efe1f82</t>
+  </si>
+  <si>
+    <t>60aa25f6fde47107c70a9fa8</t>
+  </si>
+  <si>
+    <t>60aa259212bffb07c7341ce5</t>
+  </si>
+  <si>
+    <t>60aa255675968d07c7f047c6</t>
+  </si>
+  <si>
+    <t>60aa24e0c024d307c795cbb8</t>
+  </si>
+  <si>
+    <t>60aa25ca8ede3107c711bf65</t>
+  </si>
+  <si>
+    <t>60aa2491de300707c7b1be4c</t>
+  </si>
+  <si>
+    <t>60aad5c85cdac2016efe1eca</t>
+  </si>
+  <si>
+    <t>60aad5c85cdac2016efe1f59</t>
+  </si>
+  <si>
+    <t>60aa25ca8ede3107c711bf38</t>
+  </si>
+  <si>
+    <t>2101</t>
+  </si>
+  <si>
+    <t>60aa2491de300707c7b1bf3b</t>
+  </si>
+  <si>
+    <t>201</t>
+  </si>
+  <si>
+    <t>60aa255675968d07c7f0484f</t>
+  </si>
+  <si>
+    <t>60aa25ca8ede3107c711bfab</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>60aa255675968d07c7f04910</t>
+  </si>
+  <si>
+    <t>60aa24e0c024d307c795cb7c</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,15 +259,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="70">
     <dxf>
       <font>
         <b val="0"/>
@@ -225,6 +339,60 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -306,6 +474,33 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -333,6 +528,33 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -414,6 +636,33 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -495,6 +744,33 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -522,32 +798,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -575,6 +825,221 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -602,6 +1067,60 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="1" formatCode="0"/>
       <fill>
         <patternFill patternType="none">
@@ -656,6 +1175,33 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
@@ -819,6 +1365,760 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -869,48 +2169,112 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D6B1FFB-E02A-4528-A43F-B79A6704089B}" name="Tabela1" displayName="Tabela1" ref="A1:L21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D6B1FFB-E02A-4528-A43F-B79A6704089B}" name="Tabela1" displayName="Tabela1" ref="A1:L21" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:L21" xr:uid="{FD2430C5-A63A-435D-A5DA-D7171311C5D3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
     <sortCondition ref="L1:L21"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="4" xr3:uid="{A1F90EFA-7F92-44F7-A803-A978D9117DD8}" name="CrossoverName" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{7CB4270F-7AF2-4A40-B25E-9B7CA8E5FB98}" name="Crossover.Begining" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{6DC35EC1-3E60-41C1-AEAF-2B0F474EC4AA}" name="Crossover.End" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{0D527D3E-D31D-4718-9AFC-A26B9E461682}" name="Crossover.RequiredNumberOfParents" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{57D86378-6140-429F-9022-8B6043E87E98}" name="MutationName" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{1BC565D8-2BA7-471D-B1E6-A7BBB2E4205F}" name="Mutation.AmountOfSwaps" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{8764FD96-3920-4AA6-BFA6-B59B5301A974}" name="Mutation.MutationThreshold" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{75D81516-2768-459F-A8CA-D2D1A734D00A}" name="TerminationName" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{784C77B5-B52A-4DDF-A610-44E53D50173C}" name="Termination.MaxGenerationsCount" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{C6841714-47C0-430C-8110-7DA91FDB0622}" name="Population" dataDxfId="16"/>
-    <tableColumn id="18" xr3:uid="{58B411C0-4D4D-468E-9A75-E68F00DDE616}" name="AmountOfGenerations" dataDxfId="15"/>
-    <tableColumn id="21" xr3:uid="{EE2EFF47-4ED0-4438-8ECA-699477E6BF40}" name="TotalTimeMs" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A1F90EFA-7F92-44F7-A803-A978D9117DD8}" name="CrossoverName" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{7CB4270F-7AF2-4A40-B25E-9B7CA8E5FB98}" name="Crossover.Begining" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{6DC35EC1-3E60-41C1-AEAF-2B0F474EC4AA}" name="Crossover.End" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{0D527D3E-D31D-4718-9AFC-A26B9E461682}" name="Crossover.RequiredNumberOfParents" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{57D86378-6140-429F-9022-8B6043E87E98}" name="MutationName" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{1BC565D8-2BA7-471D-B1E6-A7BBB2E4205F}" name="Mutation.AmountOfSwaps" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{8764FD96-3920-4AA6-BFA6-B59B5301A974}" name="Mutation.MutationThreshold" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{75D81516-2768-459F-A8CA-D2D1A734D00A}" name="TerminationName" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{784C77B5-B52A-4DDF-A610-44E53D50173C}" name="Termination.MaxGenerationsCount" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{C6841714-47C0-430C-8110-7DA91FDB0622}" name="Population" dataDxfId="58"/>
+    <tableColumn id="18" xr3:uid="{58B411C0-4D4D-468E-9A75-E68F00DDE616}" name="AmountOfGenerations" dataDxfId="57"/>
+    <tableColumn id="21" xr3:uid="{EE2EFF47-4ED0-4438-8ECA-699477E6BF40}" name="TotalTimeMs" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2AA4B315-9437-4299-8679-3EED117D85B4}" name="Tabela2" displayName="Tabela2" ref="A1:J21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2AA4B315-9437-4299-8679-3EED117D85B4}" name="Tabela2" displayName="Tabela2" ref="A1:J21" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
   <autoFilter ref="A1:J21" xr:uid="{8A62596E-2AB0-45F5-82A0-B51DC1F53ECF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J21">
     <sortCondition ref="J1:J21"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{D614DB4C-5B81-45CA-A4FF-DD5DC58DC5B5}" name="CrossoverName" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{332D4BDE-392F-4475-AD8D-267E8FB7E57E}" name="Crossover.Ratio" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{140C163E-8216-463A-90C8-C41606F0065F}" name="MutationName" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{DA179307-868A-4A97-A559-1A22E0875684}" name="Mutation.AmountOfSwaps" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{8AA2ECCC-AF95-4AC3-BF57-97720C93EF24}" name="Mutation.MutationThreshold" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{27F22BDF-72F3-4014-915C-24BCD5C29B72}" name="TerminationName" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{D8515C70-FBCA-41B3-A52B-FEC0CB05A238}" name="Termination.MaxGenerationsCount" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{7E6AD2C7-DBA2-44E6-AF55-99154260CE2B}" name="Population" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{88F57E62-53A1-4389-8BFB-7C3ED5ACFD67}" name="AmountOfGenerations" dataDxfId="3"/>
-    <tableColumn id="18" xr3:uid="{AF4E2C51-FDE0-4AAE-9E45-79007DAD28EE}" name="TotalTimeMs" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{D614DB4C-5B81-45CA-A4FF-DD5DC58DC5B5}" name="CrossoverName" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{332D4BDE-392F-4475-AD8D-267E8FB7E57E}" name="Crossover.Ratio" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{140C163E-8216-463A-90C8-C41606F0065F}" name="MutationName" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{DA179307-868A-4A97-A559-1A22E0875684}" name="Mutation.AmountOfSwaps" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{8AA2ECCC-AF95-4AC3-BF57-97720C93EF24}" name="Mutation.MutationThreshold" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{27F22BDF-72F3-4014-915C-24BCD5C29B72}" name="TerminationName" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{D8515C70-FBCA-41B3-A52B-FEC0CB05A238}" name="Termination.MaxGenerationsCount" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{7E6AD2C7-DBA2-44E6-AF55-99154260CE2B}" name="Population" dataDxfId="46"/>
+    <tableColumn id="15" xr3:uid="{88F57E62-53A1-4389-8BFB-7C3ED5ACFD67}" name="AmountOfGenerations" dataDxfId="45"/>
+    <tableColumn id="18" xr3:uid="{AF4E2C51-FDE0-4AAE-9E45-79007DAD28EE}" name="TotalTimeMs" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EA45784-5C9C-4C2D-82CB-5EC6510FA368}" name="Tabela3" displayName="Tabela3" ref="A1:P21" totalsRowShown="0" headerRowDxfId="26" dataDxfId="27">
+  <autoFilter ref="A1:P21" xr:uid="{21475DB6-D38F-4B05-986D-331CDF300802}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P21">
+    <sortCondition ref="P1:P21"/>
+  </sortState>
+  <tableColumns count="16">
+    <tableColumn id="2" xr3:uid="{6B063E5F-8414-462D-96AB-48A9ABA7FC05}" name="SelectionName" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{0175A4D7-CF14-4498-8567-DD1F2C373CDB}" name="Selection.IsReversed" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{9AF35E5A-B47A-4DBB-A8F4-D6197214855E}" name="Selection.HasMinus" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{887429A4-61CD-4CD4-81A3-56BA91F8999D}" name="CrossoverName" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{796C3E2C-BC6F-424D-9ECA-79CB5B67C324}" name="Crossover.Ratio" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{E1F2ED02-CDF9-4CDA-A71D-9514B29ADA01}" name="Crossover.RequiredNumberOfParents" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{9E5E2DBD-D3D6-4124-A9BF-015E0DFC73FE}" name="MutationName" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{3DA01173-BDBD-4767-A6EC-927CAF89A7F2}" name="Mutation.AmountOfSwaps" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{88C0381C-B0C0-4474-ABEE-B82B5DEB3C6F}" name="Mutation.MutationThreshold" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{F0A65C3B-2676-4E4C-AB03-9093F04B1821}" name="TerminationName" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{85693DD9-FDF4-4055-93C5-0101CCB85C7C}" name="Termination.MaxGenerationsCount" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{FEB7651A-CC1E-4D59-ACAD-EA9824590A17}" name="Population" dataDxfId="32"/>
+    <tableColumn id="15" xr3:uid="{FA2CB35C-851B-4E91-BE8D-0FD411191410}" name="AmountOfGenerations" dataDxfId="31"/>
+    <tableColumn id="16" xr3:uid="{4B1383B5-337D-40DF-90E9-DF7205087735}" name="RealTheBestValue" dataDxfId="30"/>
+    <tableColumn id="17" xr3:uid="{94AE07D7-BF17-45E6-95A5-5B943837EFC5}" name="TheBestFoundFitness" dataDxfId="29"/>
+    <tableColumn id="18" xr3:uid="{5BB522D2-0295-4289-A5D2-5BC9D669AF49}" name="TotalTimeMs" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2884EEF-0706-49BB-A7DF-1D8AE3EA6562}" name="Tabela4" displayName="Tabela4" ref="A1:X21" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:X21" xr:uid="{D176EE14-C268-4EB6-B0B3-41983DC7B972}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X21">
+    <sortCondition ref="T1:T21"/>
+  </sortState>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{43889716-B886-4014-BABE-33D064879E75}" name="_id.$oid" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{8D2C20CB-7F5C-4CE5-BFF7-976C244B97B3}" name="SelectionName" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{162FBBC7-6E87-4A92-A47D-BB316B9E877D}" name="Selection.IsReversed" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{B54AA2D6-AA93-42EE-8FB1-58636A2E1757}" name="CrossoverName" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{FF3BB4CB-F903-4DCD-AC02-C57C7D564E1B}" name="Crossover.Begining" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{FA4B3F9D-795A-4F8E-9FC1-9BC7E2096A40}" name="Crossover.End" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{9BD54C77-3C3C-49CB-B299-04644BD3CA8D}" name="Crossover.RequiredNumberOfParents" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{AACD12F1-F9BD-422A-B078-D1948C2D176D}" name="MutationName" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{B4E3E003-0045-48CC-97D4-76ED5FD15CC5}" name="Mutation.AmountOfSwaps" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{BACD1EE5-32E5-443A-B96A-81CC46534484}" name="Mutation.MutationThreshold" dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{6BB07EB3-EF8E-41D7-9D59-17E96BE713F6}" name="TerminationName" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{B3413E93-42BD-4591-BC58-D852EE9C6464}" name="Termination.AmountLastNeruonWins" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{7FCC8B77-353A-4AA3-93A6-D1F2C5692598}" name="Termination.MaxGenerationsCount" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{AC7C0F54-5463-4A2A-A6E5-1FBF2AC863E7}" name="Population" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{D82C3AB8-0D0C-4A1E-BF61-399A0A5DC1E0}" name="WinnerChromosome.TotalPath" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{DB0AE4BD-BEA5-4C3C-A3DE-E55F2932A795}" name="WinnerChromosome.Fitness" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{2608237B-2278-4EF5-B325-6873F622B12E}" name="AmountOfGenerations" dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{543DF11D-BA35-4D5F-BAF1-3FDBBBF5C4E0}" name="RealTheBestValue" dataDxfId="8"/>
+    <tableColumn id="19" xr3:uid="{82B01C31-912D-4C0F-B214-05817D8B032F}" name="TheBestFoundFitness" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{D3381EBA-1DCA-47B8-AD17-B6139CDC7086}" name="TotalTimeMs" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{FC5A3AD4-6361-47E4-B688-94152CD7A544}" name="Steps.generation" dataDxfId="5"/>
+    <tableColumn id="22" xr3:uid="{E1B9FA96-02D7-4BC2-8CCC-D30D0033766F}" name="Steps.Elapse" dataDxfId="4"/>
+    <tableColumn id="23" xr3:uid="{8B99C1F4-CFE3-4158-950E-D40C6E17B28F}" name="Steps.fitness" dataDxfId="3"/>
+    <tableColumn id="24" xr3:uid="{BC2121D5-82FF-4153-A3E7-CA3D81E1853F}" name="quality" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -2104,7 +3468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB14A026-26F2-4610-96BD-0B9792F0A3BA}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -2127,7 +3491,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -2156,7 +3520,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1">
         <v>0.2</v>
@@ -2188,7 +3552,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1">
         <v>0.2</v>
@@ -2220,7 +3584,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="1">
         <v>0.2</v>
@@ -2252,7 +3616,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>0.5</v>
@@ -2284,7 +3648,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1">
         <v>0.3</v>
@@ -2316,7 +3680,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>0.3</v>
@@ -2348,7 +3712,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <v>0.4</v>
@@ -2380,7 +3744,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>0.3</v>
@@ -2412,7 +3776,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1">
         <v>0.5</v>
@@ -2444,7 +3808,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>0.5</v>
@@ -2476,7 +3840,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>0.4</v>
@@ -2508,7 +3872,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>0.4</v>
@@ -2540,7 +3904,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14" s="1">
         <v>0.2</v>
@@ -2572,7 +3936,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1">
         <v>0.1</v>
@@ -2604,7 +3968,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
         <v>0.4</v>
@@ -2636,7 +4000,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
         <v>0.2</v>
@@ -2668,7 +4032,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>0.2</v>
@@ -2700,7 +4064,7 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>0.5</v>
@@ -2732,7 +4096,7 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B20" s="1">
         <v>0.4</v>
@@ -2764,7 +4128,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1">
         <v>0.2</v>
@@ -2813,4 +4177,2689 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95B9F0D-44EB-412E-8E72-D3ADE5904805}">
+  <dimension ref="A1:P21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.85546875" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
+    <col min="11" max="11" width="34.42578125" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" customWidth="1"/>
+    <col min="15" max="15" width="22.140625" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L2" s="2">
+        <v>100</v>
+      </c>
+      <c r="M2" s="2">
+        <v>8119</v>
+      </c>
+      <c r="N2" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O2" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P2" s="2">
+        <v>5818</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="2">
+        <v>3000</v>
+      </c>
+      <c r="L3" s="2">
+        <v>300</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3001</v>
+      </c>
+      <c r="N3" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O3" s="1">
+        <v>-1.9132230443878699</v>
+      </c>
+      <c r="P3" s="2">
+        <v>11340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L4" s="2">
+        <v>100</v>
+      </c>
+      <c r="M4" s="2">
+        <v>14457</v>
+      </c>
+      <c r="N4" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O4" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P4" s="2">
+        <v>12490</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L5" s="2">
+        <v>300</v>
+      </c>
+      <c r="M5" s="2">
+        <v>5051</v>
+      </c>
+      <c r="N5" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-1.9132230443880001</v>
+      </c>
+      <c r="P5" s="2">
+        <v>16450</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L6" s="2">
+        <v>300</v>
+      </c>
+      <c r="M6" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N6" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O6" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P6" s="2">
+        <v>25498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="2">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L7" s="2">
+        <v>300</v>
+      </c>
+      <c r="M7" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N7" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O7" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P7" s="2">
+        <v>26506</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F8" s="2">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2">
+        <v>800</v>
+      </c>
+      <c r="L8" s="2">
+        <v>300</v>
+      </c>
+      <c r="M8" s="2">
+        <v>7192</v>
+      </c>
+      <c r="N8" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O8" s="1">
+        <v>-1.9132230443880001</v>
+      </c>
+      <c r="P8" s="2">
+        <v>27696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L9" s="2">
+        <v>300</v>
+      </c>
+      <c r="M9" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N9" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O9" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P9" s="2">
+        <v>27770</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="2">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L10" s="2">
+        <v>300</v>
+      </c>
+      <c r="M10" s="2">
+        <v>8154</v>
+      </c>
+      <c r="N10" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O10" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P10" s="2">
+        <v>29044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F11" s="2">
+        <v>2</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L11" s="2">
+        <v>300</v>
+      </c>
+      <c r="M11" s="2">
+        <v>8633</v>
+      </c>
+      <c r="N11" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O11" s="1">
+        <v>-1.9132230443880001</v>
+      </c>
+      <c r="P11" s="2">
+        <v>32020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="2">
+        <v>8</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L12" s="2">
+        <v>300</v>
+      </c>
+      <c r="M12" s="2">
+        <v>12023</v>
+      </c>
+      <c r="N12" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O12" s="1">
+        <v>-1.9132230443876901</v>
+      </c>
+      <c r="P12" s="2">
+        <v>43369</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2">
+        <v>8</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="2">
+        <v>800</v>
+      </c>
+      <c r="L13" s="2">
+        <v>800</v>
+      </c>
+      <c r="M13" s="2">
+        <v>4889</v>
+      </c>
+      <c r="N13" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O13" s="1">
+        <v>-1.9132230443876601</v>
+      </c>
+      <c r="P13" s="2">
+        <v>94252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="2">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L14" s="2">
+        <v>800</v>
+      </c>
+      <c r="M14" s="2">
+        <v>7117</v>
+      </c>
+      <c r="N14" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O14" s="1">
+        <v>-1.9132230443879701</v>
+      </c>
+      <c r="P14" s="2">
+        <v>131308</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="2">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L15" s="2">
+        <v>800</v>
+      </c>
+      <c r="M15" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N15" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O15" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P15" s="2">
+        <v>144924</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F16" s="2">
+        <v>2</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L16" s="2">
+        <v>800</v>
+      </c>
+      <c r="M16" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N16" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O16" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P16" s="2">
+        <v>149612</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L17" s="2">
+        <v>800</v>
+      </c>
+      <c r="M17" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N17" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O17" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P17" s="2">
+        <v>155744</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F18" s="2">
+        <v>2</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="2">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="2">
+        <v>8000</v>
+      </c>
+      <c r="L18" s="2">
+        <v>800</v>
+      </c>
+      <c r="M18" s="2">
+        <v>8001</v>
+      </c>
+      <c r="N18" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O18" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P18" s="2">
+        <v>174089</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="2">
+        <v>8</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L19" s="2">
+        <v>800</v>
+      </c>
+      <c r="M19" s="2">
+        <v>10643</v>
+      </c>
+      <c r="N19" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O19" s="1">
+        <v>-1.9132230443880001</v>
+      </c>
+      <c r="P19" s="2">
+        <v>202244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F20" s="2">
+        <v>2</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L20" s="2">
+        <v>800</v>
+      </c>
+      <c r="M20" s="2">
+        <v>11063</v>
+      </c>
+      <c r="N20" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O20" s="1">
+        <v>-1.9132230443880001</v>
+      </c>
+      <c r="P20" s="2">
+        <v>215253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F21" s="2">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="2">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="2">
+        <v>2100</v>
+      </c>
+      <c r="L21" s="2">
+        <v>800</v>
+      </c>
+      <c r="M21" s="2">
+        <v>11187</v>
+      </c>
+      <c r="N21" s="1">
+        <v>-1.9133</v>
+      </c>
+      <c r="O21" s="1">
+        <v>-1.9132230443879299</v>
+      </c>
+      <c r="P21" s="2">
+        <v>224876</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496DF68-1D7D-4A21-89A3-FE259FA785AB}">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.7109375" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.28515625" customWidth="1"/>
+    <col min="12" max="12" width="36.28515625" customWidth="1"/>
+    <col min="13" max="13" width="34.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="30.5703125" customWidth="1"/>
+    <col min="16" max="16" width="28.42578125" customWidth="1"/>
+    <col min="17" max="17" width="23.28515625" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.5703125" customWidth="1"/>
+    <col min="21" max="21" width="18.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" customWidth="1"/>
+    <col min="24" max="24" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="2">
+        <v>200</v>
+      </c>
+      <c r="N2" s="2">
+        <v>500</v>
+      </c>
+      <c r="O2" s="1">
+        <v>33800.856034959303</v>
+      </c>
+      <c r="P2" s="1">
+        <v>33800.856034959303</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>574</v>
+      </c>
+      <c r="R2" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S2" s="1">
+        <v>33800.856034959303</v>
+      </c>
+      <c r="T2" s="2">
+        <v>2936</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1">
+        <v>122532.028895556</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1.00828851937354</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2">
+        <v>2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="2">
+        <v>800</v>
+      </c>
+      <c r="N3" s="2">
+        <v>300</v>
+      </c>
+      <c r="O3" s="1">
+        <v>33317.261652748297</v>
+      </c>
+      <c r="P3" s="1">
+        <v>33317.261652748297</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>2562</v>
+      </c>
+      <c r="R3" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S3" s="1">
+        <v>33317.261652748297</v>
+      </c>
+      <c r="T3" s="2">
+        <v>6572</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+      <c r="V3" s="2">
+        <v>2</v>
+      </c>
+      <c r="W3" s="1">
+        <v>125680.083180082</v>
+      </c>
+      <c r="X3" s="1">
+        <v>0.99386277041876503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="2">
+        <v>8000</v>
+      </c>
+      <c r="N4" s="2">
+        <v>200</v>
+      </c>
+      <c r="O4" s="1">
+        <v>34174.2238918078</v>
+      </c>
+      <c r="P4" s="1">
+        <v>34174.2238918078</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>8001</v>
+      </c>
+      <c r="R4" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S4" s="1">
+        <v>34174.2238918078</v>
+      </c>
+      <c r="T4" s="2">
+        <v>10490</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>119123.645342194</v>
+      </c>
+      <c r="X4" s="1">
+        <v>1.01942618177991</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3000</v>
+      </c>
+      <c r="N5" s="2">
+        <v>500</v>
+      </c>
+      <c r="O5" s="1">
+        <v>33668.356050951203</v>
+      </c>
+      <c r="P5" s="1">
+        <v>33668.356050951203</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>3001</v>
+      </c>
+      <c r="R5" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S5" s="1">
+        <v>33668.356050951203</v>
+      </c>
+      <c r="T5" s="2">
+        <v>15115</v>
+      </c>
+      <c r="U5" s="2">
+        <v>1</v>
+      </c>
+      <c r="V5" s="2">
+        <v>3</v>
+      </c>
+      <c r="W5" s="1">
+        <v>116581.50448857099</v>
+      </c>
+      <c r="X5" s="1">
+        <v>1.0043360096337199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="N6" s="2">
+        <v>500</v>
+      </c>
+      <c r="O6" s="1">
+        <v>34064.183159952001</v>
+      </c>
+      <c r="P6" s="1">
+        <v>34064.183159952001</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>5001</v>
+      </c>
+      <c r="R6" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S6" s="1">
+        <v>34064.183159952001</v>
+      </c>
+      <c r="T6" s="2">
+        <v>20752</v>
+      </c>
+      <c r="U6" s="2">
+        <v>1</v>
+      </c>
+      <c r="V6" s="2">
+        <v>3</v>
+      </c>
+      <c r="W6" s="1">
+        <v>125343.49586491</v>
+      </c>
+      <c r="X6" s="1">
+        <v>1.0161436375011801</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="N7" s="2">
+        <v>500</v>
+      </c>
+      <c r="O7" s="1">
+        <v>34376.419217823903</v>
+      </c>
+      <c r="P7" s="1">
+        <v>34376.419217823903</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>5001</v>
+      </c>
+      <c r="R7" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S7" s="1">
+        <v>34376.419217823903</v>
+      </c>
+      <c r="T7" s="2">
+        <v>24207</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
+        <v>3</v>
+      </c>
+      <c r="W7" s="1">
+        <v>118427.269825729</v>
+      </c>
+      <c r="X7" s="1">
+        <v>1.02545772209599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2">
+        <v>2</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M8" s="2">
+        <v>3000</v>
+      </c>
+      <c r="N8" s="2">
+        <v>800</v>
+      </c>
+      <c r="O8" s="1">
+        <v>34052.492730336802</v>
+      </c>
+      <c r="P8" s="1">
+        <v>34052.492730336802</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>3001</v>
+      </c>
+      <c r="R8" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S8" s="1">
+        <v>34052.492730336802</v>
+      </c>
+      <c r="T8" s="2">
+        <v>25362</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2">
+        <v>6</v>
+      </c>
+      <c r="W8" s="1">
+        <v>118519.45817213799</v>
+      </c>
+      <c r="X8" s="1">
+        <v>1.01579490887858</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="2">
+        <v>2100</v>
+      </c>
+      <c r="N9" s="2">
+        <v>300</v>
+      </c>
+      <c r="O9" s="1">
+        <v>34208.440921617002</v>
+      </c>
+      <c r="P9" s="1">
+        <v>34208.440921617002</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>9547</v>
+      </c>
+      <c r="R9" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S9" s="1">
+        <v>34208.440921617002</v>
+      </c>
+      <c r="T9" s="2">
+        <v>26458</v>
+      </c>
+      <c r="U9" s="2">
+        <v>1</v>
+      </c>
+      <c r="V9" s="2">
+        <v>2</v>
+      </c>
+      <c r="W9" s="1">
+        <v>120275.833422478</v>
+      </c>
+      <c r="X9" s="1">
+        <v>1.0204468848735799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2">
+        <v>2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" s="2">
+        <v>800</v>
+      </c>
+      <c r="N10" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O10" s="1">
+        <v>33527.930452444802</v>
+      </c>
+      <c r="P10" s="1">
+        <v>33527.930452444802</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1743</v>
+      </c>
+      <c r="R10" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S10" s="1">
+        <v>33527.930452444802</v>
+      </c>
+      <c r="T10" s="2">
+        <v>33989</v>
+      </c>
+      <c r="U10" s="2">
+        <v>1</v>
+      </c>
+      <c r="V10" s="2">
+        <v>8</v>
+      </c>
+      <c r="W10" s="1">
+        <v>115655.395388583</v>
+      </c>
+      <c r="X10" s="1">
+        <v>1.0001470767068801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M11" s="2">
+        <v>8000</v>
+      </c>
+      <c r="N11" s="2">
+        <v>500</v>
+      </c>
+      <c r="O11" s="1">
+        <v>33950.109949874299</v>
+      </c>
+      <c r="P11" s="1">
+        <v>33950.109949874299</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>8001</v>
+      </c>
+      <c r="R11" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S11" s="1">
+        <v>33950.109949874299</v>
+      </c>
+      <c r="T11" s="2">
+        <v>35199</v>
+      </c>
+      <c r="U11" s="2">
+        <v>1</v>
+      </c>
+      <c r="V11" s="2">
+        <v>3</v>
+      </c>
+      <c r="W11" s="1">
+        <v>120268.17552836399</v>
+      </c>
+      <c r="X11" s="1">
+        <v>1.01274080332531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G12" s="2">
+        <v>2</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="2">
+        <v>8000</v>
+      </c>
+      <c r="N12" s="2">
+        <v>500</v>
+      </c>
+      <c r="O12" s="1">
+        <v>33346.783388014701</v>
+      </c>
+      <c r="P12" s="1">
+        <v>33346.783388014701</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>8001</v>
+      </c>
+      <c r="R12" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S12" s="1">
+        <v>33346.783388014701</v>
+      </c>
+      <c r="T12" s="2">
+        <v>36942</v>
+      </c>
+      <c r="U12" s="2">
+        <v>1</v>
+      </c>
+      <c r="V12" s="2">
+        <v>3</v>
+      </c>
+      <c r="W12" s="1">
+        <v>124714.55324596001</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0.99474341162827595</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G13" s="2">
+        <v>2</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M13" s="2">
+        <v>3000</v>
+      </c>
+      <c r="N13" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O13" s="1">
+        <v>33321.5549671388</v>
+      </c>
+      <c r="P13" s="1">
+        <v>33321.5549671388</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>3001</v>
+      </c>
+      <c r="R13" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S13" s="1">
+        <v>33321.5549671388</v>
+      </c>
+      <c r="T13" s="2">
+        <v>52435</v>
+      </c>
+      <c r="U13" s="2">
+        <v>1</v>
+      </c>
+      <c r="V13" s="2">
+        <v>12</v>
+      </c>
+      <c r="W13" s="1">
+        <v>117261.643693269</v>
+      </c>
+      <c r="X13" s="1">
+        <v>0.99399084112814595</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G14" s="2">
+        <v>2</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" s="2">
+        <v>13000</v>
+      </c>
+      <c r="N14" s="2">
+        <v>500</v>
+      </c>
+      <c r="O14" s="1">
+        <v>34141.249307189399</v>
+      </c>
+      <c r="P14" s="1">
+        <v>34141.249307189399</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>13001</v>
+      </c>
+      <c r="R14" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S14" s="1">
+        <v>34141.249307189399</v>
+      </c>
+      <c r="T14" s="2">
+        <v>60670</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2">
+        <v>3</v>
+      </c>
+      <c r="W14" s="1">
+        <v>122122.144222662</v>
+      </c>
+      <c r="X14" s="1">
+        <v>1.0184425411564999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M15" s="2">
+        <v>2100</v>
+      </c>
+      <c r="N15" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O15" s="1">
+        <v>34322.407398582298</v>
+      </c>
+      <c r="P15" s="1">
+        <v>34322.407398582298</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>3612</v>
+      </c>
+      <c r="R15" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S15" s="1">
+        <v>34322.407398582298</v>
+      </c>
+      <c r="T15" s="2">
+        <v>66237</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2">
+        <v>10</v>
+      </c>
+      <c r="W15" s="1">
+        <v>120461.90380735</v>
+      </c>
+      <c r="X15" s="1">
+        <v>1.02384653517234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G16" s="2">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="2">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="N16" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O16" s="1">
+        <v>33672.665288805998</v>
+      </c>
+      <c r="P16" s="1">
+        <v>33672.665288805998</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>5001</v>
+      </c>
+      <c r="R16" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S16" s="1">
+        <v>33672.665288805998</v>
+      </c>
+      <c r="T16" s="2">
+        <v>88211</v>
+      </c>
+      <c r="U16" s="2">
+        <v>1</v>
+      </c>
+      <c r="V16" s="2">
+        <v>8</v>
+      </c>
+      <c r="W16" s="1">
+        <v>122541.79692686599</v>
+      </c>
+      <c r="X16" s="1">
+        <v>1.0044645553442699</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G17" s="2">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="N17" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O17" s="1">
+        <v>34401.848045615297</v>
+      </c>
+      <c r="P17" s="1">
+        <v>34401.848045615297</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>5001</v>
+      </c>
+      <c r="R17" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S17" s="1">
+        <v>34401.848045615297</v>
+      </c>
+      <c r="T17" s="2">
+        <v>94261</v>
+      </c>
+      <c r="U17" s="2">
+        <v>1</v>
+      </c>
+      <c r="V17" s="2">
+        <v>10</v>
+      </c>
+      <c r="W17" s="1">
+        <v>112974.278287554</v>
+      </c>
+      <c r="X17" s="1">
+        <v>1.0262162707876801</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="2">
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" s="2">
+        <v>13000</v>
+      </c>
+      <c r="N18" s="2">
+        <v>800</v>
+      </c>
+      <c r="O18" s="1">
+        <v>34364.2523702283</v>
+      </c>
+      <c r="P18" s="1">
+        <v>34364.2523702283</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>13001</v>
+      </c>
+      <c r="R18" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S18" s="1">
+        <v>34364.2523702283</v>
+      </c>
+      <c r="T18" s="2">
+        <v>124666</v>
+      </c>
+      <c r="U18" s="2">
+        <v>1</v>
+      </c>
+      <c r="V18" s="2">
+        <v>5</v>
+      </c>
+      <c r="W18" s="1">
+        <v>119976.778751773</v>
+      </c>
+      <c r="X18" s="1">
+        <v>1.02509478179842</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G19" s="2">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="2">
+        <v>3</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M19" s="2">
+        <v>13000</v>
+      </c>
+      <c r="N19" s="2">
+        <v>800</v>
+      </c>
+      <c r="O19" s="1">
+        <v>34063.731440243799</v>
+      </c>
+      <c r="P19" s="1">
+        <v>34063.731440243799</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>13001</v>
+      </c>
+      <c r="R19" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S19" s="1">
+        <v>34063.731440243799</v>
+      </c>
+      <c r="T19" s="2">
+        <v>129180</v>
+      </c>
+      <c r="U19" s="2">
+        <v>1</v>
+      </c>
+      <c r="V19" s="2">
+        <v>5</v>
+      </c>
+      <c r="W19" s="1">
+        <v>118709.81817848299</v>
+      </c>
+      <c r="X19" s="1">
+        <v>1.0161301625822201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="2">
+        <v>3</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M20" s="2">
+        <v>8000</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O20" s="1">
+        <v>33279.039836659103</v>
+      </c>
+      <c r="P20" s="1">
+        <v>33279.039836659103</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>8001</v>
+      </c>
+      <c r="R20" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S20" s="1">
+        <v>33279.039836659103</v>
+      </c>
+      <c r="T20" s="2">
+        <v>139699</v>
+      </c>
+      <c r="U20" s="2">
+        <v>1</v>
+      </c>
+      <c r="V20" s="2">
+        <v>9</v>
+      </c>
+      <c r="W20" s="1">
+        <v>117265.798874541</v>
+      </c>
+      <c r="X20" s="1">
+        <v>0.99272260348593799</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="G21" s="2">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="2">
+        <v>3</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M21" s="2">
+        <v>800</v>
+      </c>
+      <c r="N21" s="2">
+        <v>1300</v>
+      </c>
+      <c r="O21" s="1">
+        <v>34234.683881000703</v>
+      </c>
+      <c r="P21" s="1">
+        <v>34234.683881000703</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>7949</v>
+      </c>
+      <c r="R21" s="2">
+        <v>33523</v>
+      </c>
+      <c r="S21" s="1">
+        <v>34234.683881000703</v>
+      </c>
+      <c r="T21" s="2">
+        <v>153299</v>
+      </c>
+      <c r="U21" s="2">
+        <v>1</v>
+      </c>
+      <c r="V21" s="2">
+        <v>8</v>
+      </c>
+      <c r="W21" s="1">
+        <v>108673.94479120401</v>
+      </c>
+      <c r="X21" s="1">
+        <v>1.0212297193270501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Zakończono główne prace nad serią o sztucznej inteligencji.
</commit_message>
<xml_diff>
--- a/Programowanie/Sztuczna_inteligencja/problemy_i_implementacja/wyniki/Wyniki.xlsx
+++ b/Programowanie/Sztuczna_inteligencja/problemy_i_implementacja/wyniki/Wyniki.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bb75cf0a1a68a1d/Materiały pisane/Blog/Programowanie/Sztuczna_inteligencja/problemy_i_implementacja/wyniki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{28B68594-DEBB-4325-9A73-A8DA43E1A7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2E41D612-0195-4335-868B-C16147B43B8B}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{28B68594-DEBB-4325-9A73-A8DA43E1A7CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3BAA0C57-7132-45A7-A03F-5EF170943EA5}"/>
   <bookViews>
-    <workbookView xWindow="24465" yWindow="0" windowWidth="25860" windowHeight="21600" activeTab="3" xr2:uid="{9D055064-E54F-488C-B0AE-076216540D4E}"/>
+    <workbookView xWindow="25440" yWindow="8985" windowWidth="25860" windowHeight="21600" activeTab="3" xr2:uid="{9D055064-E54F-488C-B0AE-076216540D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Knapsack" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="35">
   <si>
     <t>CrossoverName</t>
   </si>
@@ -93,28 +93,7 @@
     <t>UniformCrossover`2</t>
   </si>
   <si>
-    <t>WinnerChromosome.Fitness</t>
-  </si>
-  <si>
     <t>RealTheBestValue</t>
-  </si>
-  <si>
-    <t>TheBestFoundFitness</t>
-  </si>
-  <si>
-    <t>Steps.generation</t>
-  </si>
-  <si>
-    <t>Steps.Elapse</t>
-  </si>
-  <si>
-    <t>Steps.fitness</t>
-  </si>
-  <si>
-    <t>quality</t>
-  </si>
-  <si>
-    <t>WinnerChromosome.TotalPath</t>
   </si>
   <si>
     <t/>
@@ -153,13 +132,16 @@
     <t>Amount Of Generations</t>
   </si>
   <si>
-    <t>End</t>
+    <t>Amount Last Neruon Wins</t>
   </si>
   <si>
-    <t>Begining</t>
+    <t>Crossover begining</t>
   </si>
   <si>
-    <t>Amount Last Neruon Wins</t>
+    <t>Crossover End</t>
+  </si>
+  <si>
+    <t>Total Time (ms)</t>
   </si>
 </sst>
 </file>
@@ -210,61 +192,7 @@
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
+  <dxfs count="48">
     <dxf>
       <font>
         <b val="0"/>
@@ -310,168 +238,6 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1733,96 +1499,88 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D6B1FFB-E02A-4528-A43F-B79A6704089B}" name="Tabela1" displayName="Tabela1" ref="A1:L21" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D6B1FFB-E02A-4528-A43F-B79A6704089B}" name="Tabela1" displayName="Tabela1" ref="A1:L21" totalsRowShown="0" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="A1:L21" xr:uid="{FD2430C5-A63A-435D-A5DA-D7171311C5D3}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L21">
     <sortCondition ref="L1:L21"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="4" xr3:uid="{A1F90EFA-7F92-44F7-A803-A978D9117DD8}" name="CrossoverName" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{7CB4270F-7AF2-4A40-B25E-9B7CA8E5FB98}" name="Crossover.Begining" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{6DC35EC1-3E60-41C1-AEAF-2B0F474EC4AA}" name="Crossover.End" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{0D527D3E-D31D-4718-9AFC-A26B9E461682}" name="Crossover.RequiredNumberOfParents" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{57D86378-6140-429F-9022-8B6043E87E98}" name="MutationName" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{1BC565D8-2BA7-471D-B1E6-A7BBB2E4205F}" name="Mutation.AmountOfSwaps" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{8764FD96-3920-4AA6-BFA6-B59B5301A974}" name="Mutation.MutationThreshold" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{75D81516-2768-459F-A8CA-D2D1A734D00A}" name="TerminationName" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{784C77B5-B52A-4DDF-A610-44E53D50173C}" name="Termination.MaxGenerationsCount" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{C6841714-47C0-430C-8110-7DA91FDB0622}" name="Population" dataDxfId="44"/>
-    <tableColumn id="18" xr3:uid="{58B411C0-4D4D-468E-9A75-E68F00DDE616}" name="AmountOfGenerations" dataDxfId="43"/>
-    <tableColumn id="21" xr3:uid="{EE2EFF47-4ED0-4438-8ECA-699477E6BF40}" name="TotalTimeMs" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{A1F90EFA-7F92-44F7-A803-A978D9117DD8}" name="CrossoverName" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{7CB4270F-7AF2-4A40-B25E-9B7CA8E5FB98}" name="Crossover.Begining" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{6DC35EC1-3E60-41C1-AEAF-2B0F474EC4AA}" name="Crossover.End" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{0D527D3E-D31D-4718-9AFC-A26B9E461682}" name="Crossover.RequiredNumberOfParents" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{57D86378-6140-429F-9022-8B6043E87E98}" name="MutationName" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{1BC565D8-2BA7-471D-B1E6-A7BBB2E4205F}" name="Mutation.AmountOfSwaps" dataDxfId="40"/>
+    <tableColumn id="10" xr3:uid="{8764FD96-3920-4AA6-BFA6-B59B5301A974}" name="Mutation.MutationThreshold" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{75D81516-2768-459F-A8CA-D2D1A734D00A}" name="TerminationName" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{784C77B5-B52A-4DDF-A610-44E53D50173C}" name="Termination.MaxGenerationsCount" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{C6841714-47C0-430C-8110-7DA91FDB0622}" name="Population" dataDxfId="36"/>
+    <tableColumn id="18" xr3:uid="{58B411C0-4D4D-468E-9A75-E68F00DDE616}" name="AmountOfGenerations" dataDxfId="35"/>
+    <tableColumn id="21" xr3:uid="{EE2EFF47-4ED0-4438-8ECA-699477E6BF40}" name="TotalTimeMs" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2AA4B315-9437-4299-8679-3EED117D85B4}" name="Tabela2" displayName="Tabela2" ref="A1:J21" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2AA4B315-9437-4299-8679-3EED117D85B4}" name="Tabela2" displayName="Tabela2" ref="A1:J21" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:J21" xr:uid="{8A62596E-2AB0-45F5-82A0-B51DC1F53ECF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J21">
     <sortCondition ref="J1:J21"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="5" xr3:uid="{D614DB4C-5B81-45CA-A4FF-DD5DC58DC5B5}" name="CrossoverName" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{332D4BDE-392F-4475-AD8D-267E8FB7E57E}" name="Crossover.Ratio" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{140C163E-8216-463A-90C8-C41606F0065F}" name="MutationName" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{DA179307-868A-4A97-A559-1A22E0875684}" name="Mutation.AmountOfSwaps" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{8AA2ECCC-AF95-4AC3-BF57-97720C93EF24}" name="Mutation.MutationThreshold" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{27F22BDF-72F3-4014-915C-24BCD5C29B72}" name="TerminationName" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{D8515C70-FBCA-41B3-A52B-FEC0CB05A238}" name="Termination.MaxGenerationsCount" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{7E6AD2C7-DBA2-44E6-AF55-99154260CE2B}" name="Population" dataDxfId="32"/>
-    <tableColumn id="15" xr3:uid="{88F57E62-53A1-4389-8BFB-7C3ED5ACFD67}" name="AmountOfGenerations" dataDxfId="31"/>
-    <tableColumn id="18" xr3:uid="{AF4E2C51-FDE0-4AAE-9E45-79007DAD28EE}" name="TotalTimeMs" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{D614DB4C-5B81-45CA-A4FF-DD5DC58DC5B5}" name="CrossoverName" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{332D4BDE-392F-4475-AD8D-267E8FB7E57E}" name="Crossover.Ratio" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{140C163E-8216-463A-90C8-C41606F0065F}" name="MutationName" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{DA179307-868A-4A97-A559-1A22E0875684}" name="Mutation.AmountOfSwaps" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{8AA2ECCC-AF95-4AC3-BF57-97720C93EF24}" name="Mutation.MutationThreshold" dataDxfId="27"/>
+    <tableColumn id="11" xr3:uid="{27F22BDF-72F3-4014-915C-24BCD5C29B72}" name="TerminationName" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{D8515C70-FBCA-41B3-A52B-FEC0CB05A238}" name="Termination.MaxGenerationsCount" dataDxfId="25"/>
+    <tableColumn id="13" xr3:uid="{7E6AD2C7-DBA2-44E6-AF55-99154260CE2B}" name="Population" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{88F57E62-53A1-4389-8BFB-7C3ED5ACFD67}" name="AmountOfGenerations" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{AF4E2C51-FDE0-4AAE-9E45-79007DAD28EE}" name="TotalTimeMs" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EA45784-5C9C-4C2D-82CB-5EC6510FA368}" name="Tabela3" displayName="Tabela3" ref="A1:H21" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2EA45784-5C9C-4C2D-82CB-5EC6510FA368}" name="Tabela3" displayName="Tabela3" ref="A1:H21" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:H21" xr:uid="{21475DB6-D38F-4B05-986D-331CDF300802}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H21">
     <sortCondition ref="H1:H21"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="6" xr3:uid="{796C3E2C-BC6F-424D-9ECA-79CB5B67C324}" name="Ratio" dataDxfId="27"/>
-    <tableColumn id="9" xr3:uid="{3DA01173-BDBD-4767-A6EC-927CAF89A7F2}" name="Amount Of Swaps" dataDxfId="26"/>
-    <tableColumn id="10" xr3:uid="{88C0381C-B0C0-4474-ABEE-B82B5DEB3C6F}" name="Mutation Threshold" dataDxfId="25"/>
-    <tableColumn id="11" xr3:uid="{F0A65C3B-2676-4E4C-AB03-9093F04B1821}" name="Termination Name" dataDxfId="24"/>
-    <tableColumn id="12" xr3:uid="{85693DD9-FDF4-4055-93C5-0101CCB85C7C}" name="Max Generations Count" dataDxfId="23"/>
-    <tableColumn id="13" xr3:uid="{FEB7651A-CC1E-4D59-ACAD-EA9824590A17}" name="Population" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{FA2CB35C-851B-4E91-BE8D-0FD411191410}" name="Amount Of Generations" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{5BB522D2-0295-4289-A5D2-5BC9D669AF49}" name="TotalTimeMs" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{796C3E2C-BC6F-424D-9ECA-79CB5B67C324}" name="Ratio" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{3DA01173-BDBD-4767-A6EC-927CAF89A7F2}" name="Amount Of Swaps" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{88C0381C-B0C0-4474-ABEE-B82B5DEB3C6F}" name="Mutation Threshold" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{F0A65C3B-2676-4E4C-AB03-9093F04B1821}" name="Termination Name" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{85693DD9-FDF4-4055-93C5-0101CCB85C7C}" name="Max Generations Count" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{FEB7651A-CC1E-4D59-ACAD-EA9824590A17}" name="Population" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{FA2CB35C-851B-4E91-BE8D-0FD411191410}" name="Amount Of Generations" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{5BB522D2-0295-4289-A5D2-5BC9D669AF49}" name="TotalTimeMs" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2884EEF-0706-49BB-A7DF-1D8AE3EA6562}" name="Tabela4" displayName="Tabela4" ref="A1:R21" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R21" xr:uid="{D176EE14-C268-4EB6-B0B3-41983DC7B972}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R21">
-    <sortCondition ref="N1:N21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D2884EEF-0706-49BB-A7DF-1D8AE3EA6562}" name="Tabela4" displayName="Tabela4" ref="A1:J21" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J21" xr:uid="{D176EE14-C268-4EB6-B0B3-41983DC7B972}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J21">
+    <sortCondition ref="J1:J21"/>
   </sortState>
-  <tableColumns count="18">
-    <tableColumn id="5" xr3:uid="{FF3BB4CB-F903-4DCD-AC02-C57C7D564E1B}" name="Begining" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{FA4B3F9D-795A-4F8E-9FC1-9BC7E2096A40}" name="End" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{B4E3E003-0045-48CC-97D4-76ED5FD15CC5}" name="Amount Of Swaps" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{BACD1EE5-32E5-443A-B96A-81CC46534484}" name="Mutation Threshold" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{6BB07EB3-EF8E-41D7-9D59-17E96BE713F6}" name="TerminationName" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{B3413E93-42BD-4591-BC58-D852EE9C6464}" name="Amount Last Neruon Wins" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{7FCC8B77-353A-4AA3-93A6-D1F2C5692598}" name="Max Generations Count" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{AC7C0F54-5463-4A2A-A6E5-1FBF2AC863E7}" name="Population" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{D82C3AB8-0D0C-4A1E-BF61-399A0A5DC1E0}" name="WinnerChromosome.TotalPath" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{DB0AE4BD-BEA5-4C3C-A3DE-E55F2932A795}" name="WinnerChromosome.Fitness" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{2608237B-2278-4EF5-B325-6873F622B12E}" name="AmountOfGenerations" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{543DF11D-BA35-4D5F-BAF1-3FDBBBF5C4E0}" name="RealTheBestValue" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{82B01C31-912D-4C0F-B214-05817D8B032F}" name="TheBestFoundFitness" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{D3381EBA-1DCA-47B8-AD17-B6139CDC7086}" name="TotalTimeMs" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{FC5A3AD4-6361-47E4-B688-94152CD7A544}" name="Steps.generation" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{E1B9FA96-02D7-4BC2-8CCC-D30D0033766F}" name="Steps.Elapse" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{8B99C1F4-CFE3-4158-950E-D40C6E17B28F}" name="Steps.fitness" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{BC2121D5-82FF-4153-A3E7-CA3D81E1853F}" name="quality" dataDxfId="0"/>
+  <tableColumns count="10">
+    <tableColumn id="5" xr3:uid="{FF3BB4CB-F903-4DCD-AC02-C57C7D564E1B}" name="Crossover begining" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{FA4B3F9D-795A-4F8E-9FC1-9BC7E2096A40}" name="Crossover End" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{B4E3E003-0045-48CC-97D4-76ED5FD15CC5}" name="Amount Of Swaps" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{BACD1EE5-32E5-443A-B96A-81CC46534484}" name="Mutation Threshold" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{6BB07EB3-EF8E-41D7-9D59-17E96BE713F6}" name="TerminationName" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{B3413E93-42BD-4591-BC58-D852EE9C6464}" name="Amount Last Neruon Wins" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{7FCC8B77-353A-4AA3-93A6-D1F2C5692598}" name="Max Generations Count" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{AC7C0F54-5463-4A2A-A6E5-1FBF2AC863E7}" name="Population" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{2608237B-2278-4EF5-B325-6873F622B12E}" name="Amount Of Generations" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{D3381EBA-1DCA-47B8-AD17-B6139CDC7086}" name="Total Time (ms)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3752,31 +3510,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -3790,7 +3548,7 @@
         <v>0.2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E2" s="2">
         <v>2100</v>
@@ -3819,7 +3577,7 @@
         <v>0.4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2">
         <v>3000</v>
@@ -3848,7 +3606,7 @@
         <v>0.9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2">
         <v>2100</v>
@@ -3877,7 +3635,7 @@
         <v>0.4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E5" s="2">
         <v>2100</v>
@@ -3906,7 +3664,7 @@
         <v>0.5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2">
         <v>8000</v>
@@ -3935,7 +3693,7 @@
         <v>0.4</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2">
         <v>8000</v>
@@ -3964,7 +3722,7 @@
         <v>0.7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2">
         <v>800</v>
@@ -3993,7 +3751,7 @@
         <v>0.4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2">
         <v>8000</v>
@@ -4022,7 +3780,7 @@
         <v>0.5</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2">
         <v>2100</v>
@@ -4051,7 +3809,7 @@
         <v>0.7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2">
         <v>2100</v>
@@ -4080,7 +3838,7 @@
         <v>0.5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E12" s="2">
         <v>2100</v>
@@ -4109,7 +3867,7 @@
         <v>0.7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E13" s="2">
         <v>800</v>
@@ -4138,7 +3896,7 @@
         <v>0.2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E14" s="2">
         <v>2100</v>
@@ -4167,7 +3925,7 @@
         <v>0.5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E15" s="2">
         <v>8000</v>
@@ -4196,7 +3954,7 @@
         <v>0.4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E16" s="2">
         <v>8000</v>
@@ -4225,7 +3983,7 @@
         <v>0.4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2">
         <v>8000</v>
@@ -4254,7 +4012,7 @@
         <v>0.9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E18" s="2">
         <v>8000</v>
@@ -4283,7 +4041,7 @@
         <v>0.2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2">
         <v>2100</v>
@@ -4312,7 +4070,7 @@
         <v>0.2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E20" s="2">
         <v>2100</v>
@@ -4341,7 +4099,7 @@
         <v>0.4</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E21" s="2">
         <v>2100</v>
@@ -4371,10 +4129,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9496DF68-1D7D-4A21-89A3-FE259FA785AB}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4387,75 +4145,43 @@
     <col min="6" max="6" width="36.28515625" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.28515625" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="14" max="14" width="14.5703125" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.1</v>
       </c>
@@ -4469,10 +4195,10 @@
         <v>0.9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="G2" s="2">
         <v>200</v>
@@ -4480,38 +4206,14 @@
       <c r="H2" s="2">
         <v>500</v>
       </c>
-      <c r="I2" s="1">
-        <v>33800.856034959303</v>
-      </c>
-      <c r="J2" s="1">
-        <v>33800.856034959303</v>
-      </c>
-      <c r="K2" s="2">
+      <c r="I2" s="2">
         <v>574</v>
       </c>
-      <c r="L2" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M2" s="1">
-        <v>33800.856034959303</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="J2" s="2">
         <v>2936</v>
       </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>122532.028895556</v>
-      </c>
-      <c r="R2" s="1">
-        <v>1.00828851937354</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.3</v>
       </c>
@@ -4525,10 +4227,10 @@
         <v>0.9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2">
         <v>800</v>
@@ -4536,38 +4238,14 @@
       <c r="H3" s="2">
         <v>300</v>
       </c>
-      <c r="I3" s="1">
-        <v>33317.261652748297</v>
-      </c>
-      <c r="J3" s="1">
-        <v>33317.261652748297</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="I3" s="2">
         <v>2562</v>
       </c>
-      <c r="L3" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M3" s="1">
-        <v>33317.261652748297</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="J3" s="2">
         <v>6572</v>
       </c>
-      <c r="O3" s="2">
-        <v>1</v>
-      </c>
-      <c r="P3" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>125680.083180082</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0.99386277041876503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.4</v>
       </c>
@@ -4581,10 +4259,10 @@
         <v>0.9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G4" s="2">
         <v>8000</v>
@@ -4592,38 +4270,14 @@
       <c r="H4" s="2">
         <v>200</v>
       </c>
-      <c r="I4" s="1">
-        <v>34174.2238918078</v>
-      </c>
-      <c r="J4" s="1">
-        <v>34174.2238918078</v>
-      </c>
-      <c r="K4" s="2">
+      <c r="I4" s="2">
         <v>8001</v>
       </c>
-      <c r="L4" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M4" s="1">
-        <v>34174.2238918078</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="J4" s="2">
         <v>10490</v>
       </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
-      <c r="P4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>119123.645342194</v>
-      </c>
-      <c r="R4" s="1">
-        <v>1.01942618177991</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.1</v>
       </c>
@@ -4637,10 +4291,10 @@
         <v>0.6</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G5" s="2">
         <v>3000</v>
@@ -4648,38 +4302,14 @@
       <c r="H5" s="2">
         <v>500</v>
       </c>
-      <c r="I5" s="1">
-        <v>33668.356050951203</v>
-      </c>
-      <c r="J5" s="1">
-        <v>33668.356050951203</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="I5" s="2">
         <v>3001</v>
       </c>
-      <c r="L5" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M5" s="1">
-        <v>33668.356050951203</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="J5" s="2">
         <v>15115</v>
       </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
-      <c r="P5" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>116581.50448857099</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1.0043360096337199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.4</v>
       </c>
@@ -4693,10 +4323,10 @@
         <v>0.7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2">
         <v>5000</v>
@@ -4704,38 +4334,14 @@
       <c r="H6" s="2">
         <v>500</v>
       </c>
-      <c r="I6" s="1">
-        <v>34064.183159952001</v>
-      </c>
-      <c r="J6" s="1">
-        <v>34064.183159952001</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="I6" s="2">
         <v>5001</v>
       </c>
-      <c r="L6" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M6" s="1">
-        <v>34064.183159952001</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="J6" s="2">
         <v>20752</v>
       </c>
-      <c r="O6" s="2">
-        <v>1</v>
-      </c>
-      <c r="P6" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>125343.49586491</v>
-      </c>
-      <c r="R6" s="1">
-        <v>1.0161436375011801</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.2</v>
       </c>
@@ -4749,10 +4355,10 @@
         <v>0.5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G7" s="2">
         <v>5000</v>
@@ -4760,38 +4366,14 @@
       <c r="H7" s="2">
         <v>500</v>
       </c>
-      <c r="I7" s="1">
-        <v>34376.419217823903</v>
-      </c>
-      <c r="J7" s="1">
-        <v>34376.419217823903</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="I7" s="2">
         <v>5001</v>
       </c>
-      <c r="L7" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M7" s="1">
-        <v>34376.419217823903</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="J7" s="2">
         <v>24207</v>
       </c>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>118427.269825729</v>
-      </c>
-      <c r="R7" s="1">
-        <v>1.02545772209599</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.4</v>
       </c>
@@ -4805,10 +4387,10 @@
         <v>0.8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G8" s="2">
         <v>3000</v>
@@ -4816,38 +4398,14 @@
       <c r="H8" s="2">
         <v>800</v>
       </c>
-      <c r="I8" s="1">
-        <v>34052.492730336802</v>
-      </c>
-      <c r="J8" s="1">
-        <v>34052.492730336802</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="I8" s="2">
         <v>3001</v>
       </c>
-      <c r="L8" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M8" s="1">
-        <v>34052.492730336802</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="J8" s="2">
         <v>25362</v>
       </c>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
-      <c r="P8" s="2">
-        <v>6</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>118519.45817213799</v>
-      </c>
-      <c r="R8" s="1">
-        <v>1.01579490887858</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.2</v>
       </c>
@@ -4861,10 +4419,10 @@
         <v>0.7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G9" s="2">
         <v>2100</v>
@@ -4872,38 +4430,14 @@
       <c r="H9" s="2">
         <v>300</v>
       </c>
-      <c r="I9" s="1">
-        <v>34208.440921617002</v>
-      </c>
-      <c r="J9" s="1">
-        <v>34208.440921617002</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="I9" s="2">
         <v>9547</v>
       </c>
-      <c r="L9" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M9" s="1">
-        <v>34208.440921617002</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="J9" s="2">
         <v>26458</v>
       </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>120275.833422478</v>
-      </c>
-      <c r="R9" s="1">
-        <v>1.0204468848735799</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.2</v>
       </c>
@@ -4917,10 +4451,10 @@
         <v>0.9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2">
         <v>800</v>
@@ -4928,38 +4462,14 @@
       <c r="H10" s="2">
         <v>1300</v>
       </c>
-      <c r="I10" s="1">
-        <v>33527.930452444802</v>
-      </c>
-      <c r="J10" s="1">
-        <v>33527.930452444802</v>
-      </c>
-      <c r="K10" s="2">
+      <c r="I10" s="2">
         <v>1743</v>
       </c>
-      <c r="L10" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M10" s="1">
-        <v>33527.930452444802</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="J10" s="2">
         <v>33989</v>
       </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
-      <c r="P10" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>115655.395388583</v>
-      </c>
-      <c r="R10" s="1">
-        <v>1.0001470767068801</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.3</v>
       </c>
@@ -4973,10 +4483,10 @@
         <v>0.3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2">
         <v>8000</v>
@@ -4984,38 +4494,14 @@
       <c r="H11" s="2">
         <v>500</v>
       </c>
-      <c r="I11" s="1">
-        <v>33950.109949874299</v>
-      </c>
-      <c r="J11" s="1">
-        <v>33950.109949874299</v>
-      </c>
-      <c r="K11" s="2">
+      <c r="I11" s="2">
         <v>8001</v>
       </c>
-      <c r="L11" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M11" s="1">
-        <v>33950.109949874299</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="J11" s="2">
         <v>35199</v>
       </c>
-      <c r="O11" s="2">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>120268.17552836399</v>
-      </c>
-      <c r="R11" s="1">
-        <v>1.01274080332531</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.3</v>
       </c>
@@ -5029,10 +4515,10 @@
         <v>0.8</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G12" s="2">
         <v>8000</v>
@@ -5040,38 +4526,14 @@
       <c r="H12" s="2">
         <v>500</v>
       </c>
-      <c r="I12" s="1">
-        <v>33346.783388014701</v>
-      </c>
-      <c r="J12" s="1">
-        <v>33346.783388014701</v>
-      </c>
-      <c r="K12" s="2">
+      <c r="I12" s="2">
         <v>8001</v>
       </c>
-      <c r="L12" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M12" s="1">
-        <v>33346.783388014701</v>
-      </c>
-      <c r="N12" s="2">
+      <c r="J12" s="2">
         <v>36942</v>
       </c>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
-      <c r="P12" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="1">
-        <v>124714.55324596001</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0.99474341162827595</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.4</v>
       </c>
@@ -5085,10 +4547,10 @@
         <v>0.6</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G13" s="2">
         <v>3000</v>
@@ -5096,38 +4558,14 @@
       <c r="H13" s="2">
         <v>1300</v>
       </c>
-      <c r="I13" s="1">
-        <v>33321.5549671388</v>
-      </c>
-      <c r="J13" s="1">
-        <v>33321.5549671388</v>
-      </c>
-      <c r="K13" s="2">
+      <c r="I13" s="2">
         <v>3001</v>
       </c>
-      <c r="L13" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M13" s="1">
-        <v>33321.5549671388</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="J13" s="2">
         <v>52435</v>
       </c>
-      <c r="O13" s="2">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2">
-        <v>12</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>117261.643693269</v>
-      </c>
-      <c r="R13" s="1">
-        <v>0.99399084112814595</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.3</v>
       </c>
@@ -5141,10 +4579,10 @@
         <v>0.8</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G14" s="2">
         <v>13000</v>
@@ -5152,38 +4590,14 @@
       <c r="H14" s="2">
         <v>500</v>
       </c>
-      <c r="I14" s="1">
-        <v>34141.249307189399</v>
-      </c>
-      <c r="J14" s="1">
-        <v>34141.249307189399</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="I14" s="2">
         <v>13001</v>
       </c>
-      <c r="L14" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M14" s="1">
-        <v>34141.249307189399</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="J14" s="2">
         <v>60670</v>
       </c>
-      <c r="O14" s="2">
-        <v>1</v>
-      </c>
-      <c r="P14" s="2">
-        <v>3</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>122122.144222662</v>
-      </c>
-      <c r="R14" s="1">
-        <v>1.0184425411564999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.3</v>
       </c>
@@ -5197,10 +4611,10 @@
         <v>0.7</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G15" s="2">
         <v>2100</v>
@@ -5208,38 +4622,14 @@
       <c r="H15" s="2">
         <v>1300</v>
       </c>
-      <c r="I15" s="1">
-        <v>34322.407398582298</v>
-      </c>
-      <c r="J15" s="1">
-        <v>34322.407398582298</v>
-      </c>
-      <c r="K15" s="2">
+      <c r="I15" s="2">
         <v>3612</v>
       </c>
-      <c r="L15" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M15" s="1">
-        <v>34322.407398582298</v>
-      </c>
-      <c r="N15" s="2">
+      <c r="J15" s="2">
         <v>66237</v>
       </c>
-      <c r="O15" s="2">
-        <v>1</v>
-      </c>
-      <c r="P15" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>120461.90380735</v>
-      </c>
-      <c r="R15" s="1">
-        <v>1.02384653517234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.4</v>
       </c>
@@ -5253,10 +4643,10 @@
         <v>0.9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2">
         <v>5000</v>
@@ -5264,38 +4654,14 @@
       <c r="H16" s="2">
         <v>1300</v>
       </c>
-      <c r="I16" s="1">
-        <v>33672.665288805998</v>
-      </c>
-      <c r="J16" s="1">
-        <v>33672.665288805998</v>
-      </c>
-      <c r="K16" s="2">
+      <c r="I16" s="2">
         <v>5001</v>
       </c>
-      <c r="L16" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M16" s="1">
-        <v>33672.665288805998</v>
-      </c>
-      <c r="N16" s="2">
+      <c r="J16" s="2">
         <v>88211</v>
       </c>
-      <c r="O16" s="2">
-        <v>1</v>
-      </c>
-      <c r="P16" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>122541.79692686599</v>
-      </c>
-      <c r="R16" s="1">
-        <v>1.0044645553442699</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.2</v>
       </c>
@@ -5309,10 +4675,10 @@
         <v>0.3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G17" s="2">
         <v>5000</v>
@@ -5320,38 +4686,14 @@
       <c r="H17" s="2">
         <v>1300</v>
       </c>
-      <c r="I17" s="1">
-        <v>34401.848045615297</v>
-      </c>
-      <c r="J17" s="1">
-        <v>34401.848045615297</v>
-      </c>
-      <c r="K17" s="2">
+      <c r="I17" s="2">
         <v>5001</v>
       </c>
-      <c r="L17" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M17" s="1">
-        <v>34401.848045615297</v>
-      </c>
-      <c r="N17" s="2">
+      <c r="J17" s="2">
         <v>94261</v>
       </c>
-      <c r="O17" s="2">
-        <v>1</v>
-      </c>
-      <c r="P17" s="2">
-        <v>10</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>112974.278287554</v>
-      </c>
-      <c r="R17" s="1">
-        <v>1.0262162707876801</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.2</v>
       </c>
@@ -5365,10 +4707,10 @@
         <v>0.5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G18" s="2">
         <v>13000</v>
@@ -5376,38 +4718,14 @@
       <c r="H18" s="2">
         <v>800</v>
       </c>
-      <c r="I18" s="1">
-        <v>34364.2523702283</v>
-      </c>
-      <c r="J18" s="1">
-        <v>34364.2523702283</v>
-      </c>
-      <c r="K18" s="2">
+      <c r="I18" s="2">
         <v>13001</v>
       </c>
-      <c r="L18" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M18" s="1">
-        <v>34364.2523702283</v>
-      </c>
-      <c r="N18" s="2">
+      <c r="J18" s="2">
         <v>124666</v>
       </c>
-      <c r="O18" s="2">
-        <v>1</v>
-      </c>
-      <c r="P18" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>119976.778751773</v>
-      </c>
-      <c r="R18" s="1">
-        <v>1.02509478179842</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.1</v>
       </c>
@@ -5421,10 +4739,10 @@
         <v>0.4</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G19" s="2">
         <v>13000</v>
@@ -5432,38 +4750,14 @@
       <c r="H19" s="2">
         <v>800</v>
       </c>
-      <c r="I19" s="1">
-        <v>34063.731440243799</v>
-      </c>
-      <c r="J19" s="1">
-        <v>34063.731440243799</v>
-      </c>
-      <c r="K19" s="2">
+      <c r="I19" s="2">
         <v>13001</v>
       </c>
-      <c r="L19" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M19" s="1">
-        <v>34063.731440243799</v>
-      </c>
-      <c r="N19" s="2">
+      <c r="J19" s="2">
         <v>129180</v>
       </c>
-      <c r="O19" s="2">
-        <v>1</v>
-      </c>
-      <c r="P19" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>118709.81817848299</v>
-      </c>
-      <c r="R19" s="1">
-        <v>1.0161301625822201</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.4</v>
       </c>
@@ -5477,10 +4771,10 @@
         <v>0.4</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="G20" s="2">
         <v>8000</v>
@@ -5488,38 +4782,14 @@
       <c r="H20" s="2">
         <v>1300</v>
       </c>
-      <c r="I20" s="1">
-        <v>33279.039836659103</v>
-      </c>
-      <c r="J20" s="1">
-        <v>33279.039836659103</v>
-      </c>
-      <c r="K20" s="2">
+      <c r="I20" s="2">
         <v>8001</v>
       </c>
-      <c r="L20" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M20" s="1">
-        <v>33279.039836659103</v>
-      </c>
-      <c r="N20" s="2">
+      <c r="J20" s="2">
         <v>139699</v>
       </c>
-      <c r="O20" s="2">
-        <v>1</v>
-      </c>
-      <c r="P20" s="2">
-        <v>9</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>117265.798874541</v>
-      </c>
-      <c r="R20" s="1">
-        <v>0.99272260348593799</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.1</v>
       </c>
@@ -5533,10 +4803,10 @@
         <v>0.3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G21" s="2">
         <v>800</v>
@@ -5544,41 +4814,18 @@
       <c r="H21" s="2">
         <v>1300</v>
       </c>
-      <c r="I21" s="1">
-        <v>34234.683881000703</v>
-      </c>
-      <c r="J21" s="1">
-        <v>34234.683881000703</v>
-      </c>
-      <c r="K21" s="2">
+      <c r="I21" s="2">
         <v>7949</v>
       </c>
-      <c r="L21" s="2">
-        <v>33523</v>
-      </c>
-      <c r="M21" s="1">
-        <v>34234.683881000703</v>
-      </c>
-      <c r="N21" s="2">
+      <c r="J21" s="2">
         <v>153299</v>
-      </c>
-      <c r="O21" s="2">
-        <v>1</v>
-      </c>
-      <c r="P21" s="2">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>108673.94479120401</v>
-      </c>
-      <c r="R21" s="1">
-        <v>1.0212297193270501</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>